<commit_message>
Functional streaming (memcpy and kernel launch)
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\ece408-21fa\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39DD641-576C-499C-933C-DCC004C1A2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3549CC6-47E8-4497-8E28-78F28C07B572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1092" yWindow="804" windowWidth="22116" windowHeight="10932" xr2:uid="{3EBBDD75-A876-4BC2-A19F-83F1058A81CD}"/>
+    <workbookView xWindow="1020" yWindow="804" windowWidth="22116" windowHeight="10932" xr2:uid="{3EBBDD75-A876-4BC2-A19F-83F1058A81CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -200,10 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,6 +211,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,102 +536,108 @@
   <dimension ref="B2:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C13" sqref="C13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="6"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="1"/>
       <c r="F3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
       <c r="F4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
       <c r="F6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
+      <c r="B7" s="6"/>
       <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="8"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
@@ -638,31 +645,34 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
       <c r="F10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
@@ -670,25 +680,25 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F14" t="s">
@@ -696,25 +706,25 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F16" t="s">

</xml_diff>

<commit_message>
Backup streaming code to archive
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\ece408-21fa\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3549CC6-47E8-4497-8E28-78F28C07B572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0ACCBA-D603-445C-ABE9-D13B59730195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="804" windowWidth="22116" windowHeight="10932" xr2:uid="{3EBBDD75-A876-4BC2-A19F-83F1058A81CD}"/>
+    <workbookView xWindow="924" yWindow="804" windowWidth="22116" windowHeight="10932" xr2:uid="{3EBBDD75-A876-4BC2-A19F-83F1058A81CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +120,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -213,6 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +543,7 @@
   <dimension ref="B2:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +690,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="4" t="s">
         <v>14</v>
       </c>

</xml_diff>